<commit_message>
Adjustment in the Config.xlsx file.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\753493\Documents\UiPath\RPAChallenge\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7112335F-4B84-4542-A96F-D73FD013FE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19271E3C-FE6B-4ED5-BB3F-F87D6E327473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="-11640" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>ListOfPeople</t>
+  </si>
+  <si>
+    <t>Stores the path where the Base file will be stored.</t>
+  </si>
+  <si>
+    <t>Link to download the Base file. (Default value: https://www.rpachallenge.com/assets/downloadFiles/challenge.xlsx)</t>
   </si>
 </sst>
 </file>
@@ -547,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2794,8 +2800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2852,6 +2858,9 @@
       <c r="C2" t="s">
         <v>45</v>
       </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
@@ -2862,6 +2871,9 @@
       </c>
       <c r="C3" t="s">
         <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>